<commit_message>
Melhorias na batalha e TM
</commit_message>
<xml_diff>
--- a/Data/ItemCard.xlsx
+++ b/Data/ItemCard.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="16635" windowHeight="11475"/>
+    <workbookView windowWidth="13020" windowHeight="12645" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Standard" sheetId="1" r:id="rId1"/>
+    <sheet name="Main" sheetId="1" r:id="rId1"/>
+    <sheet name="TM" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="389">
   <si>
     <t>ID</t>
   </si>
@@ -671,6 +672,609 @@
   </si>
   <si>
     <t>Bicicleta</t>
+  </si>
+  <si>
+    <t>Gen</t>
+  </si>
+  <si>
+    <t>HM 01</t>
+  </si>
+  <si>
+    <t>M.TM.148</t>
+  </si>
+  <si>
+    <t>VI</t>
+  </si>
+  <si>
+    <t>HM 02</t>
+  </si>
+  <si>
+    <t>M.TM.158</t>
+  </si>
+  <si>
+    <t>HM 03</t>
+  </si>
+  <si>
+    <t>M.TM.159</t>
+  </si>
+  <si>
+    <t>HM 04</t>
+  </si>
+  <si>
+    <t>M.TM.160</t>
+  </si>
+  <si>
+    <t>HM 05</t>
+  </si>
+  <si>
+    <t>M.TM.135</t>
+  </si>
+  <si>
+    <t>HM 06</t>
+  </si>
+  <si>
+    <t>M.TM.161</t>
+  </si>
+  <si>
+    <t>HM 07</t>
+  </si>
+  <si>
+    <t>M.TM.162</t>
+  </si>
+  <si>
+    <t>TM 01</t>
+  </si>
+  <si>
+    <t>M.TM.163</t>
+  </si>
+  <si>
+    <t>TM 02</t>
+  </si>
+  <si>
+    <t>M.TM.164</t>
+  </si>
+  <si>
+    <t>TM 03</t>
+  </si>
+  <si>
+    <t>M.TM.82</t>
+  </si>
+  <si>
+    <t>TM 04</t>
+  </si>
+  <si>
+    <t>M.TM.170</t>
+  </si>
+  <si>
+    <t>TM 05</t>
+  </si>
+  <si>
+    <t>M.TM.78</t>
+  </si>
+  <si>
+    <t>TM 06</t>
+  </si>
+  <si>
+    <t>M.TM.102</t>
+  </si>
+  <si>
+    <t>TM 07</t>
+  </si>
+  <si>
+    <t>M.TM.171</t>
+  </si>
+  <si>
+    <t>TM 08</t>
+  </si>
+  <si>
+    <t>M.TM.172</t>
+  </si>
+  <si>
+    <t>TM 09</t>
+  </si>
+  <si>
+    <t>M.TM.22</t>
+  </si>
+  <si>
+    <t>TM 10</t>
+  </si>
+  <si>
+    <t>M.TM.173</t>
+  </si>
+  <si>
+    <t>TM 11</t>
+  </si>
+  <si>
+    <t>M.TM.175</t>
+  </si>
+  <si>
+    <t>TM 41</t>
+  </si>
+  <si>
+    <t>M.TM.176</t>
+  </si>
+  <si>
+    <t>TM 12</t>
+  </si>
+  <si>
+    <t>M.TM.177</t>
+  </si>
+  <si>
+    <t>TM 13</t>
+  </si>
+  <si>
+    <t>M.TM.100</t>
+  </si>
+  <si>
+    <t>TM 14</t>
+  </si>
+  <si>
+    <t>M.TM.154</t>
+  </si>
+  <si>
+    <t>TM 15</t>
+  </si>
+  <si>
+    <t>M.TM.94</t>
+  </si>
+  <si>
+    <t>TM 16</t>
+  </si>
+  <si>
+    <t>M.TM.117</t>
+  </si>
+  <si>
+    <t>TM 17</t>
+  </si>
+  <si>
+    <t>M.TM.179</t>
+  </si>
+  <si>
+    <t>TM 18</t>
+  </si>
+  <si>
+    <t>M.TM.15</t>
+  </si>
+  <si>
+    <t>TM 19</t>
+  </si>
+  <si>
+    <t>M.TM.180</t>
+  </si>
+  <si>
+    <t>TM 20</t>
+  </si>
+  <si>
+    <t>M.TM.165</t>
+  </si>
+  <si>
+    <t>TM 21</t>
+  </si>
+  <si>
+    <t>M.TM.166</t>
+  </si>
+  <si>
+    <t>TM 22</t>
+  </si>
+  <si>
+    <t>M.TM.6</t>
+  </si>
+  <si>
+    <t>TM 23</t>
+  </si>
+  <si>
+    <t>M.TM.88</t>
+  </si>
+  <si>
+    <t>TM 24</t>
+  </si>
+  <si>
+    <t>M.TM.96</t>
+  </si>
+  <si>
+    <t>TM 25</t>
+  </si>
+  <si>
+    <t>M.TM.181</t>
+  </si>
+  <si>
+    <t>TM 26</t>
+  </si>
+  <si>
+    <t>M.TM.70</t>
+  </si>
+  <si>
+    <t>TM 27</t>
+  </si>
+  <si>
+    <t>M.TM.167</t>
+  </si>
+  <si>
+    <t>TM 28</t>
+  </si>
+  <si>
+    <t>M.TM.48</t>
+  </si>
+  <si>
+    <t>TM 29</t>
+  </si>
+  <si>
+    <t>M.TM.112</t>
+  </si>
+  <si>
+    <t>TM 30</t>
+  </si>
+  <si>
+    <t>M.TM.109</t>
+  </si>
+  <si>
+    <t>TM 31</t>
+  </si>
+  <si>
+    <t>M.TM.168</t>
+  </si>
+  <si>
+    <t>TM 32</t>
+  </si>
+  <si>
+    <t>M.TM.169</t>
+  </si>
+  <si>
+    <t>TM 33</t>
+  </si>
+  <si>
+    <t>M.TM.183</t>
+  </si>
+  <si>
+    <t>TM 34</t>
+  </si>
+  <si>
+    <t>M.TM.65</t>
+  </si>
+  <si>
+    <t>TM 35</t>
+  </si>
+  <si>
+    <t>M.TM.9</t>
+  </si>
+  <si>
+    <t>TM 36</t>
+  </si>
+  <si>
+    <t>M.TM.127</t>
+  </si>
+  <si>
+    <t>TM 37</t>
+  </si>
+  <si>
+    <t>M.TM.184</t>
+  </si>
+  <si>
+    <t>TM 38</t>
+  </si>
+  <si>
+    <t>M.TM.11</t>
+  </si>
+  <si>
+    <t>TM 39</t>
+  </si>
+  <si>
+    <t>M.TM.185</t>
+  </si>
+  <si>
+    <t>TM 40</t>
+  </si>
+  <si>
+    <t>M.TM.186</t>
+  </si>
+  <si>
+    <t>TM 42</t>
+  </si>
+  <si>
+    <t>M.TM.187</t>
+  </si>
+  <si>
+    <t>TM 43</t>
+  </si>
+  <si>
+    <t>M.TM.188</t>
+  </si>
+  <si>
+    <t>TM 45</t>
+  </si>
+  <si>
+    <t>M.TM.190</t>
+  </si>
+  <si>
+    <t>TM 46</t>
+  </si>
+  <si>
+    <t>M.TM.189</t>
+  </si>
+  <si>
+    <t>TM 47</t>
+  </si>
+  <si>
+    <t>M.TM.76</t>
+  </si>
+  <si>
+    <t>TM 48</t>
+  </si>
+  <si>
+    <t>M.TM.191</t>
+  </si>
+  <si>
+    <t>TM 49</t>
+  </si>
+  <si>
+    <t>M.TM.192</t>
+  </si>
+  <si>
+    <t>TM 50</t>
+  </si>
+  <si>
+    <t>M.TM.193</t>
+  </si>
+  <si>
+    <t>TM 51</t>
+  </si>
+  <si>
+    <t>M.TM.182</t>
+  </si>
+  <si>
+    <t>TM 52</t>
+  </si>
+  <si>
+    <t>M.TM.194</t>
+  </si>
+  <si>
+    <t>TM 53</t>
+  </si>
+  <si>
+    <t>M.TM.195</t>
+  </si>
+  <si>
+    <t>TM 54</t>
+  </si>
+  <si>
+    <t>M.TM.196</t>
+  </si>
+  <si>
+    <t>TM 55</t>
+  </si>
+  <si>
+    <t>M.TM.133</t>
+  </si>
+  <si>
+    <t>TM 57</t>
+  </si>
+  <si>
+    <t>M.TM.197</t>
+  </si>
+  <si>
+    <t>TM 58</t>
+  </si>
+  <si>
+    <t>M.TM.198</t>
+  </si>
+  <si>
+    <t>TM 59</t>
+  </si>
+  <si>
+    <t>M.TM.199</t>
+  </si>
+  <si>
+    <t>TM 60</t>
+  </si>
+  <si>
+    <t>M.TM.200</t>
+  </si>
+  <si>
+    <t>TM 61</t>
+  </si>
+  <si>
+    <t>M.TM.201</t>
+  </si>
+  <si>
+    <t>TM 62</t>
+  </si>
+  <si>
+    <t>M.TM.202</t>
+  </si>
+  <si>
+    <t>TM 63</t>
+  </si>
+  <si>
+    <t>M.TM.203</t>
+  </si>
+  <si>
+    <t>TM 64</t>
+  </si>
+  <si>
+    <t>M.TM.116</t>
+  </si>
+  <si>
+    <t>TM 65</t>
+  </si>
+  <si>
+    <t>M.TM.204</t>
+  </si>
+  <si>
+    <t>TM 66</t>
+  </si>
+  <si>
+    <t>M.TM.205</t>
+  </si>
+  <si>
+    <t>TM 67</t>
+  </si>
+  <si>
+    <t>M.TM.206</t>
+  </si>
+  <si>
+    <t>TM 68</t>
+  </si>
+  <si>
+    <t>M.TM.207</t>
+  </si>
+  <si>
+    <t>TM 69</t>
+  </si>
+  <si>
+    <t>M.TM.208</t>
+  </si>
+  <si>
+    <t>TM 71</t>
+  </si>
+  <si>
+    <t>M.TM.129</t>
+  </si>
+  <si>
+    <t>TM 72</t>
+  </si>
+  <si>
+    <t>M.TM.209</t>
+  </si>
+  <si>
+    <t>TM 73</t>
+  </si>
+  <si>
+    <t>M.TM.146</t>
+  </si>
+  <si>
+    <t>TM 74</t>
+  </si>
+  <si>
+    <t>M.TM.210</t>
+  </si>
+  <si>
+    <t>TM 75</t>
+  </si>
+  <si>
+    <t>M.TM.97</t>
+  </si>
+  <si>
+    <t>TM 76</t>
+  </si>
+  <si>
+    <t>M.TM.211</t>
+  </si>
+  <si>
+    <t>TM 78</t>
+  </si>
+  <si>
+    <t>M.TM.87</t>
+  </si>
+  <si>
+    <t>TM 79</t>
+  </si>
+  <si>
+    <t>M.TM.212</t>
+  </si>
+  <si>
+    <t>TM 80</t>
+  </si>
+  <si>
+    <t>M.TM.111</t>
+  </si>
+  <si>
+    <t>TM 81</t>
+  </si>
+  <si>
+    <t>M.TM.139</t>
+  </si>
+  <si>
+    <t>TM 82</t>
+  </si>
+  <si>
+    <t>M.TM.213</t>
+  </si>
+  <si>
+    <t>TM 83</t>
+  </si>
+  <si>
+    <t>M.TM.214</t>
+  </si>
+  <si>
+    <t>TM 84</t>
+  </si>
+  <si>
+    <t>M.TM.215</t>
+  </si>
+  <si>
+    <t>TM 85</t>
+  </si>
+  <si>
+    <t>M.TM.157</t>
+  </si>
+  <si>
+    <t>TM 86</t>
+  </si>
+  <si>
+    <t>M.TM.216</t>
+  </si>
+  <si>
+    <t>TM 87</t>
+  </si>
+  <si>
+    <t>M.TM.217</t>
+  </si>
+  <si>
+    <t>TM 88</t>
+  </si>
+  <si>
+    <t>M.TM.218</t>
+  </si>
+  <si>
+    <t>TM 89</t>
+  </si>
+  <si>
+    <t>M.TM.219</t>
+  </si>
+  <si>
+    <t>TM 91</t>
+  </si>
+  <si>
+    <t>M.TM.220</t>
+  </si>
+  <si>
+    <t>TM 93</t>
+  </si>
+  <si>
+    <t>M.TM.221</t>
+  </si>
+  <si>
+    <t>TM 94</t>
+  </si>
+  <si>
+    <t>TM 95</t>
+  </si>
+  <si>
+    <t>M.TM.222</t>
+  </si>
+  <si>
+    <t>TM 96</t>
+  </si>
+  <si>
+    <t>M.TM.223</t>
+  </si>
+  <si>
+    <t>TM 97</t>
+  </si>
+  <si>
+    <t>M.TM.108</t>
+  </si>
+  <si>
+    <t>TM 98</t>
+  </si>
+  <si>
+    <t>M.TM.225</t>
+  </si>
+  <si>
+    <t>TM 99</t>
+  </si>
+  <si>
+    <t>M.TM.226</t>
   </si>
 </sst>
 </file>
@@ -1299,13 +1903,20 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1387,13 +1998,7 @@
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabela1" displayName="Tabela1" ref="A1:G45" totalsRowShown="0">
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G45" etc:filterBottomFollowUsedRange="0">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="Catch"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G45" etc:filterBottomFollowUsedRange="0"/>
   <sortState ref="A1:G45">
     <sortCondition ref="A1"/>
   </sortState>
@@ -1405,6 +2010,22 @@
     <tableColumn id="7" name="Rarity"/>
     <tableColumn id="4" name="Description" dataDxfId="3"/>
     <tableColumn id="6" name="Name PT"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabela1_3" displayName="Tabela1_3" ref="A1:D101" totalsRowShown="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:D101" etc:filterBottomFollowUsedRange="0"/>
+  <sortState ref="A1:D101">
+    <sortCondition ref="A1:A45"/>
+  </sortState>
+  <tableColumns count="4">
+    <tableColumn id="1" name="ID"/>
+    <tableColumn id="2" name="Name"/>
+    <tableColumn id="4" name="Effect"/>
+    <tableColumn id="5" name="Gen"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1670,8 +2291,8 @@
   <sheetPr/>
   <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D49" sqref="D49"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="G1" sqref="A1:G45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="6"/>
@@ -1709,7 +2330,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" ht="45" hidden="1" spans="1:7">
+    <row r="2" ht="45" spans="1:7">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -1732,7 +2353,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" hidden="1" spans="1:7">
+    <row r="3" spans="1:7">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -1755,7 +2376,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="4" hidden="1" spans="1:7">
+    <row r="4" spans="1:7">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -1778,7 +2399,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" hidden="1" spans="1:7">
+    <row r="5" spans="1:7">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -1801,7 +2422,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" hidden="1" spans="1:7">
+    <row r="6" spans="1:7">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1824,7 +2445,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" hidden="1" spans="1:7">
+    <row r="7" spans="1:7">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1847,7 +2468,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" hidden="1" spans="1:7">
+    <row r="8" spans="1:7">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1870,7 +2491,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="9" ht="30" hidden="1" spans="1:7">
+    <row r="9" ht="30" spans="1:7">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1893,7 +2514,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="10" ht="45" hidden="1" spans="1:7">
+    <row r="10" ht="45" spans="1:7">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1916,7 +2537,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" ht="30" hidden="1" spans="1:7">
+    <row r="11" ht="30" spans="1:7">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1939,7 +2560,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" ht="30" hidden="1" spans="1:7">
+    <row r="12" ht="30" spans="1:7">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1962,7 +2583,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" ht="45" hidden="1" spans="1:7">
+    <row r="13" ht="45" spans="1:7">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1985,7 +2606,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="14" ht="45" hidden="1" spans="1:7">
+    <row r="14" ht="45" spans="1:7">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -2001,14 +2622,14 @@
       <c r="E14" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F14" s="3" t="s">
+      <c r="F14" s="6" t="s">
         <v>63</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="15" ht="45" hidden="1" spans="1:7">
+    <row r="15" ht="45" spans="1:7">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -2024,14 +2645,14 @@
       <c r="E15" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="6" t="s">
         <v>67</v>
       </c>
       <c r="G15" s="1" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="16" ht="45" hidden="1" spans="1:7">
+    <row r="16" ht="45" spans="1:7">
       <c r="A16" s="1">
         <v>15</v>
       </c>
@@ -2047,14 +2668,14 @@
       <c r="E16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="3" t="s">
+      <c r="F16" s="6" t="s">
         <v>71</v>
       </c>
       <c r="G16" s="1" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="17" ht="45" hidden="1" spans="1:7">
+    <row r="17" ht="45" spans="1:7">
       <c r="A17" s="1">
         <v>16</v>
       </c>
@@ -2070,14 +2691,14 @@
       <c r="E17" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="F17" s="3" t="s">
+      <c r="F17" s="6" t="s">
         <v>75</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="18" ht="30" hidden="1" spans="1:7">
+    <row r="18" ht="30" spans="1:7">
       <c r="A18" s="1">
         <v>17</v>
       </c>
@@ -2100,7 +2721,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="19" ht="30" hidden="1" spans="1:7">
+    <row r="19" ht="30" spans="1:7">
       <c r="A19" s="1">
         <v>18</v>
       </c>
@@ -2123,7 +2744,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="20" ht="30" hidden="1" spans="1:7">
+    <row r="20" ht="30" spans="1:7">
       <c r="A20" s="1">
         <v>19</v>
       </c>
@@ -2146,7 +2767,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" ht="30" hidden="1" spans="1:7">
+    <row r="21" ht="30" spans="1:7">
       <c r="A21" s="1">
         <v>20</v>
       </c>
@@ -2169,7 +2790,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="22" ht="30" hidden="1" spans="1:7">
+    <row r="22" ht="30" spans="1:7">
       <c r="A22" s="1">
         <v>21</v>
       </c>
@@ -2192,7 +2813,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="23" ht="30" hidden="1" spans="1:7">
+    <row r="23" ht="30" spans="1:7">
       <c r="A23" s="1">
         <v>22</v>
       </c>
@@ -2215,7 +2836,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" ht="30" hidden="1" spans="1:7">
+    <row r="24" ht="30" spans="1:7">
       <c r="A24" s="1">
         <v>23</v>
       </c>
@@ -2238,7 +2859,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="25" ht="45" hidden="1" spans="1:7">
+    <row r="25" ht="45" spans="1:7">
       <c r="A25" s="1">
         <v>24</v>
       </c>
@@ -2261,7 +2882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" ht="30" hidden="1" spans="1:7">
+    <row r="26" ht="30" spans="1:7">
       <c r="A26" s="1">
         <v>25</v>
       </c>
@@ -2284,7 +2905,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="27" ht="45" hidden="1" spans="1:7">
+    <row r="27" ht="45" spans="1:7">
       <c r="A27" s="1">
         <v>26</v>
       </c>
@@ -2307,7 +2928,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="28" ht="30" hidden="1" spans="1:7">
+    <row r="28" ht="30" spans="1:7">
       <c r="A28" s="1">
         <v>27</v>
       </c>
@@ -2330,7 +2951,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="29" ht="30" hidden="1" spans="1:7">
+    <row r="29" ht="30" spans="1:7">
       <c r="A29" s="1">
         <v>28</v>
       </c>
@@ -2353,7 +2974,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="30" ht="30" hidden="1" spans="1:7">
+    <row r="30" ht="30" spans="1:7">
       <c r="A30" s="1">
         <v>29</v>
       </c>
@@ -2376,7 +2997,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="31" ht="30" hidden="1" spans="1:7">
+    <row r="31" ht="30" spans="1:7">
       <c r="A31" s="1">
         <v>30</v>
       </c>
@@ -2399,7 +3020,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="32" hidden="1" spans="1:7">
+    <row r="32" spans="1:7">
       <c r="A32" s="1">
         <v>31</v>
       </c>
@@ -2560,7 +3181,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="39" hidden="1" spans="1:7">
+    <row r="39" spans="1:7">
       <c r="A39" s="1">
         <v>38</v>
       </c>
@@ -2583,7 +3204,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="40" hidden="1" spans="1:7">
+    <row r="40" spans="1:7">
       <c r="A40" s="1">
         <v>39</v>
       </c>
@@ -2606,7 +3227,7 @@
         <v>166</v>
       </c>
     </row>
-    <row r="41" hidden="1" spans="1:7">
+    <row r="41" spans="1:7">
       <c r="A41" s="1">
         <v>40</v>
       </c>
@@ -2629,7 +3250,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="42" hidden="1" spans="1:7">
+    <row r="42" spans="1:7">
       <c r="A42" s="1">
         <v>41</v>
       </c>
@@ -2652,7 +3273,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="43" hidden="1" spans="1:7">
+    <row r="43" spans="1:7">
       <c r="A43" s="1">
         <v>42</v>
       </c>
@@ -2675,7 +3296,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="44" hidden="1" spans="1:7">
+    <row r="44" spans="1:7">
       <c r="A44" s="1" t="s">
         <v>181</v>
       </c>
@@ -2695,7 +3316,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="45" ht="30" hidden="1" spans="1:7">
+    <row r="45" ht="30" spans="1:7">
       <c r="A45" s="1" t="s">
         <v>181</v>
       </c>
@@ -2722,4 +3343,1459 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D104"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="205" zoomScaleNormal="205" topLeftCell="A87" workbookViewId="0">
+      <selection activeCell="C91" sqref="C91"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="4.71428571428571" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
+    <col min="3" max="3" width="10.1428571428571" customWidth="1"/>
+    <col min="4" max="4" width="5.28571428571429" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>199</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>205</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="1">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" s="1">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" s="1">
+        <v>12</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" s="1">
+        <v>13</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" s="1">
+        <v>14</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>216</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>217</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" s="1">
+        <v>15</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" s="1">
+        <v>16</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="1">
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>222</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" s="1">
+        <v>18</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>224</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" s="1">
+        <v>19</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>226</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" s="1">
+        <v>20</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D21" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" s="1">
+        <v>21</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="D22" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" s="1">
+        <v>22</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>232</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="D23" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" s="1">
+        <v>23</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>234</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="D24" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" s="1">
+        <v>24</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>236</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="D25" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" s="1">
+        <v>25</v>
+      </c>
+      <c r="B26" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D26" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" s="1">
+        <v>26</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" s="1">
+        <v>27</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" s="1">
+        <v>28</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>244</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" s="1">
+        <v>29</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="D30" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" s="1">
+        <v>30</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D31" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" s="1">
+        <v>31</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" s="1">
+        <v>32</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" s="1">
+        <v>33</v>
+      </c>
+      <c r="B34" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" s="1">
+        <v>34</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" s="1">
+        <v>35</v>
+      </c>
+      <c r="B36" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" s="1">
+        <v>36</v>
+      </c>
+      <c r="B37" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>261</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" s="1">
+        <v>37</v>
+      </c>
+      <c r="B38" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>263</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" s="1">
+        <v>38</v>
+      </c>
+      <c r="B39" s="1" t="s">
+        <v>264</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>265</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" s="1">
+        <v>39</v>
+      </c>
+      <c r="B40" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>267</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" s="1">
+        <v>40</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>269</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="1">
+        <v>41</v>
+      </c>
+      <c r="B42" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>271</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="1">
+        <v>42</v>
+      </c>
+      <c r="B43" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="1">
+        <v>43</v>
+      </c>
+      <c r="B44" s="1" t="s">
+        <v>274</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="D44" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="1">
+        <v>44</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="D45" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="1">
+        <v>45</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C46" t="s">
+        <v>279</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="1">
+        <v>46</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="C47" t="s">
+        <v>281</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="1">
+        <v>47</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="C48" t="s">
+        <v>283</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="1">
+        <v>48</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>284</v>
+      </c>
+      <c r="C49" t="s">
+        <v>285</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="1">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>287</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="1">
+        <v>50</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>289</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="1">
+        <v>51</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="C52" s="4" t="s">
+        <v>291</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="1">
+        <v>52</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="1">
+        <v>53</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="C54" s="4" t="s">
+        <v>295</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="1">
+        <v>54</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="C55" s="4" t="s">
+        <v>297</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="1">
+        <v>55</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="C56" s="4" t="s">
+        <v>299</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="1">
+        <v>56</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>301</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="1">
+        <v>57</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>303</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="1">
+        <v>58</v>
+      </c>
+      <c r="B59" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="C59" t="s">
+        <v>305</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="1">
+        <v>59</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="C60" t="s">
+        <v>307</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="1">
+        <v>60</v>
+      </c>
+      <c r="B61" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="C61" t="s">
+        <v>309</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="1">
+        <v>61</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C62" t="s">
+        <v>311</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="1">
+        <v>62</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="C63" t="s">
+        <v>313</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="1">
+        <v>63</v>
+      </c>
+      <c r="B64" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="C64" t="s">
+        <v>315</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="1">
+        <v>64</v>
+      </c>
+      <c r="B65" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C65" t="s">
+        <v>317</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="1">
+        <v>65</v>
+      </c>
+      <c r="B66" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C66" t="s">
+        <v>319</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="1">
+        <v>66</v>
+      </c>
+      <c r="B67" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C67" t="s">
+        <v>321</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="1">
+        <v>67</v>
+      </c>
+      <c r="B68" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="C68" t="s">
+        <v>323</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="A69" s="1">
+        <v>68</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="C69" t="s">
+        <v>325</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4">
+      <c r="A70" s="1">
+        <v>69</v>
+      </c>
+      <c r="B70" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="C70" t="s">
+        <v>327</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4">
+      <c r="A71" s="1">
+        <v>70</v>
+      </c>
+      <c r="B71" s="3" t="s">
+        <v>328</v>
+      </c>
+      <c r="C71" t="s">
+        <v>329</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4">
+      <c r="A72" s="1">
+        <v>71</v>
+      </c>
+      <c r="B72" s="3" t="s">
+        <v>330</v>
+      </c>
+      <c r="C72" t="s">
+        <v>331</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4">
+      <c r="A73" s="1">
+        <v>72</v>
+      </c>
+      <c r="B73" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="C73" t="s">
+        <v>333</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4">
+      <c r="A74" s="1">
+        <v>73</v>
+      </c>
+      <c r="B74" s="3" t="s">
+        <v>334</v>
+      </c>
+      <c r="C74" t="s">
+        <v>335</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4">
+      <c r="A75" s="1">
+        <v>74</v>
+      </c>
+      <c r="B75" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="C75" t="s">
+        <v>337</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4">
+      <c r="A76" s="1">
+        <v>75</v>
+      </c>
+      <c r="B76" s="3" t="s">
+        <v>338</v>
+      </c>
+      <c r="C76" t="s">
+        <v>339</v>
+      </c>
+      <c r="D76" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4">
+      <c r="A77" s="1">
+        <v>76</v>
+      </c>
+      <c r="B77" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="C77" t="s">
+        <v>341</v>
+      </c>
+      <c r="D77" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4">
+      <c r="A78" s="1">
+        <v>77</v>
+      </c>
+      <c r="B78" s="3" t="s">
+        <v>342</v>
+      </c>
+      <c r="C78" t="s">
+        <v>343</v>
+      </c>
+      <c r="D78" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4">
+      <c r="A79" s="1">
+        <v>78</v>
+      </c>
+      <c r="B79" s="3" t="s">
+        <v>344</v>
+      </c>
+      <c r="C79" t="s">
+        <v>345</v>
+      </c>
+      <c r="D79" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4">
+      <c r="A80" s="1">
+        <v>79</v>
+      </c>
+      <c r="B80" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="C80" t="s">
+        <v>347</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4">
+      <c r="A81" s="1">
+        <v>80</v>
+      </c>
+      <c r="B81" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="C81" t="s">
+        <v>349</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4">
+      <c r="A82" s="1">
+        <v>81</v>
+      </c>
+      <c r="B82" s="3" t="s">
+        <v>350</v>
+      </c>
+      <c r="C82" t="s">
+        <v>351</v>
+      </c>
+      <c r="D82" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4">
+      <c r="A83" s="1">
+        <v>82</v>
+      </c>
+      <c r="B83" s="3" t="s">
+        <v>352</v>
+      </c>
+      <c r="C83" t="s">
+        <v>353</v>
+      </c>
+      <c r="D83" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4">
+      <c r="A84" s="1">
+        <v>83</v>
+      </c>
+      <c r="B84" s="3" t="s">
+        <v>354</v>
+      </c>
+      <c r="C84" t="s">
+        <v>355</v>
+      </c>
+      <c r="D84" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4">
+      <c r="A85" s="1">
+        <v>84</v>
+      </c>
+      <c r="B85" s="3" t="s">
+        <v>356</v>
+      </c>
+      <c r="C85" t="s">
+        <v>357</v>
+      </c>
+      <c r="D85" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4">
+      <c r="A86" s="1">
+        <v>85</v>
+      </c>
+      <c r="B86" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="C86" t="s">
+        <v>359</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4">
+      <c r="A87" s="1">
+        <v>86</v>
+      </c>
+      <c r="B87" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="C87" t="s">
+        <v>361</v>
+      </c>
+      <c r="D87" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4">
+      <c r="A88" s="1">
+        <v>87</v>
+      </c>
+      <c r="B88" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="C88" t="s">
+        <v>363</v>
+      </c>
+      <c r="D88" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4">
+      <c r="A89" s="1">
+        <v>88</v>
+      </c>
+      <c r="B89" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="C89" t="s">
+        <v>365</v>
+      </c>
+      <c r="D89" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4">
+      <c r="A90" s="1">
+        <v>89</v>
+      </c>
+      <c r="B90" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="C90" t="s">
+        <v>367</v>
+      </c>
+      <c r="D90" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4">
+      <c r="A91" s="1">
+        <v>90</v>
+      </c>
+      <c r="B91" s="3" t="s">
+        <v>368</v>
+      </c>
+      <c r="C91" t="s">
+        <v>369</v>
+      </c>
+      <c r="D91" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4">
+      <c r="A92" s="1">
+        <v>91</v>
+      </c>
+      <c r="B92" s="3" t="s">
+        <v>370</v>
+      </c>
+      <c r="C92" t="s">
+        <v>371</v>
+      </c>
+      <c r="D92" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="93" spans="1:4">
+      <c r="A93" s="1">
+        <v>92</v>
+      </c>
+      <c r="B93" s="3" t="s">
+        <v>372</v>
+      </c>
+      <c r="C93" t="s">
+        <v>373</v>
+      </c>
+      <c r="D93" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="94" spans="1:4">
+      <c r="A94" s="1">
+        <v>93</v>
+      </c>
+      <c r="B94" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="C94" t="s">
+        <v>375</v>
+      </c>
+      <c r="D94" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4">
+      <c r="A95" s="1">
+        <v>94</v>
+      </c>
+      <c r="B95" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="C95" t="s">
+        <v>377</v>
+      </c>
+      <c r="D95" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4">
+      <c r="A96" s="1">
+        <v>95</v>
+      </c>
+      <c r="B96" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="C96" t="s">
+        <v>223</v>
+      </c>
+      <c r="D96" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4">
+      <c r="A97" s="1">
+        <v>96</v>
+      </c>
+      <c r="B97" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="C97" t="s">
+        <v>380</v>
+      </c>
+      <c r="D97" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4">
+      <c r="A98" s="1">
+        <v>97</v>
+      </c>
+      <c r="B98" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="C98" t="s">
+        <v>382</v>
+      </c>
+      <c r="D98" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4">
+      <c r="A99" s="1">
+        <v>98</v>
+      </c>
+      <c r="B99" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="C99" t="s">
+        <v>384</v>
+      </c>
+      <c r="D99" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4">
+      <c r="A100" s="1">
+        <v>99</v>
+      </c>
+      <c r="B100" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="C100" t="s">
+        <v>386</v>
+      </c>
+      <c r="D100" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="101" spans="1:4">
+      <c r="A101" s="1">
+        <v>100</v>
+      </c>
+      <c r="B101" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="C101" t="s">
+        <v>388</v>
+      </c>
+      <c r="D101" s="1" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="102" spans="1:4">
+      <c r="A102" s="1"/>
+      <c r="B102" s="5"/>
+      <c r="D102" s="1"/>
+    </row>
+    <row r="103" spans="1:4">
+      <c r="A103" s="1"/>
+      <c r="B103" s="5"/>
+      <c r="D103" s="1"/>
+    </row>
+    <row r="104" spans="1:4">
+      <c r="A104" s="1"/>
+      <c r="B104" s="3"/>
+      <c r="D104" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>